<commit_message>
WIP generate_nama_sbu, generate_df_single_sbu dan report_template
</commit_message>
<xml_diff>
--- a/report_template.xlsx
+++ b/report_template.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ProjectInGit\pri_retail_daily_sales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9FB2EE-5A26-4BBB-ABB8-71E64DDFB359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8652929C-5A9E-420D-A498-DBF30F29AEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2085" yWindow="2640" windowWidth="21600" windowHeight="11835" firstSheet="1" activeTab="3" xr2:uid="{32CC4FEA-9B44-457B-A0AE-E1E6A0050CC1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{32CC4FEA-9B44-457B-A0AE-E1E6A0050CC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard SBU" sheetId="1" r:id="rId1"/>
     <sheet name="Dashboard Area" sheetId="2" r:id="rId2"/>
     <sheet name="Dashboard Comp &amp; Non Comp Store" sheetId="3" r:id="rId3"/>
     <sheet name="Our Daily Dose" sheetId="7" r:id="rId4"/>
-    <sheet name="Fisik" sheetId="4" r:id="rId5"/>
-    <sheet name="Bazaar" sheetId="5" r:id="rId6"/>
+    <sheet name="Fisik" sheetId="8" r:id="rId5"/>
+    <sheet name="Bazaar" sheetId="9" r:id="rId6"/>
     <sheet name="Detail Daily Sales &amp; Est." sheetId="6" r:id="rId7"/>
   </sheets>
   <externalReferences>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
   <si>
     <t>{{ title }}</t>
   </si>
@@ -111,6 +111,18 @@
   </si>
   <si>
     <t>{{ df_odd | noheader }}</t>
+  </si>
+  <si>
+    <t>{{ df_fisik | noheader }}</t>
+  </si>
+  <si>
+    <t>{{ df_bazaar | noheader }}</t>
+  </si>
+  <si>
+    <t>{{ judul_bazaar }}</t>
+  </si>
+  <si>
+    <t>{{ judul_fisik }}</t>
   </si>
 </sst>
 </file>
@@ -120,9 +132,9 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="\R\p\ #,##0.00,,\ \j\t"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +165,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -255,20 +275,8 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -278,6 +286,28 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -318,7 +348,7 @@
       <sheetData sheetId="1">
         <row r="2">
           <cell r="F2">
-            <v>45327</v>
+            <v>45337</v>
           </cell>
         </row>
       </sheetData>
@@ -682,129 +712,127 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0.85546875" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" style="11" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="7" customWidth="1"/>
+    <col min="8" max="9" width="15.7109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="6" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" style="7" customWidth="1"/>
+    <col min="13" max="14" width="15.7109375" style="6" customWidth="1"/>
+    <col min="15" max="15" width="16.5703125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" style="6" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" style="7" customWidth="1"/>
     <col min="18" max="18" width="0.85546875" customWidth="1"/>
     <col min="19" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7" t="s">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
     </row>
     <row r="4" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -823,25 +851,287 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30785F4F-FF33-4D48-88BB-944465766AD2}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A62E3C6-A6D5-4EB3-8083-9E513FD6B6DE}">
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:D1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="0.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" style="11" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="7" customWidth="1"/>
+    <col min="8" max="9" width="15.7109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="6" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" style="7" customWidth="1"/>
+    <col min="13" max="14" width="15.7109375" style="6" customWidth="1"/>
+    <col min="15" max="15" width="16.5703125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" style="6" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" style="7" customWidth="1"/>
+    <col min="18" max="18" width="0.85546875" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+    </row>
+    <row r="4" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="M3:Q3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA242EB-FF07-4B68-A7D4-CE3ED4C044F5}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C3B8A6-BA18-4F95-9615-1FEB88D7E73E}">
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:D1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="0.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" style="11" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="7" customWidth="1"/>
+    <col min="8" max="9" width="15.7109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="6" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" style="7" customWidth="1"/>
+    <col min="13" max="14" width="15.7109375" style="6" customWidth="1"/>
+    <col min="15" max="15" width="16.5703125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" style="6" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" style="7" customWidth="1"/>
+    <col min="18" max="18" width="0.85546875" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+    </row>
+    <row r="4" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="M3:Q3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>